<commit_message>
Updated few failed test cases of Regression test run
</commit_message>
<xml_diff>
--- a/Test Data/Verify Trip Current Calculation for Multiple Base.xlsx
+++ b/Test Data/Verify Trip Current Calculation for Multiple Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D72BE-7622-4136-8D2D-E9E531A404BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A470CD06-30E9-4F2E-9A20-D9FC6312A40E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices Loop A" sheetId="6" r:id="rId1"/>
@@ -303,13 +303,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,12 +610,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="F1" s="3" t="s">
         <v>24</v>
       </c>
@@ -631,10 +631,10 @@
       <c r="B2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="16"/>
       <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
@@ -833,7 +833,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,16 +850,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="4"/>
@@ -871,15 +871,15 @@
       <c r="B2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="16"/>
       <c r="F2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="5">
-        <v>449.5</v>
+        <v>427.2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -897,7 +897,7 @@
         <v>41</v>
       </c>
       <c r="G3" s="5">
-        <v>449.5</v>
+        <v>427.2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,16 +1082,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="4"/>
@@ -1103,15 +1103,15 @@
       <c r="B2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="16"/>
       <c r="F2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="5">
-        <v>370.6</v>
+        <v>360.6</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1129,7 +1129,7 @@
         <v>41</v>
       </c>
       <c r="G3" s="5">
-        <v>354.6</v>
+        <v>344.6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1247,7 +1247,7 @@
         <v>30</v>
       </c>
       <c r="J9" s="8">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated Test data for Verify Trip Current Calculation for Multiple Base
</commit_message>
<xml_diff>
--- a/Test Data/Verify Trip Current Calculation for Multiple Base.xlsx
+++ b/Test Data/Verify Trip Current Calculation for Multiple Base.xlsx
@@ -31,8 +31,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alpesh Dhakad</author>
+  </authors>
+  <commentList>
+    <comment ref="I9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+4B 4" [517.050.041] &amp; 801HL</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>Device</t>
   </si>
@@ -127,9 +161,6 @@
     <t>Isolator Jumper On</t>
   </si>
   <si>
-    <t>4B 4" [517.050.041] &amp; 801HL</t>
-  </si>
-  <si>
     <t>DC Units on UI for changing base of 850PH</t>
   </si>
   <si>
@@ -197,13 +228,16 @@
   </si>
   <si>
     <t>Current (worst case)</t>
+  </si>
+  <si>
+    <t>Assign Base/Default Base Row Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +259,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -597,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,7 +679,7 @@
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -640,7 +687,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>10</v>
@@ -653,7 +700,7 @@
         <v>338.9</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -661,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="12" t="s">
@@ -674,7 +721,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -682,7 +729,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="12" t="s">
@@ -701,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5">
         <v>378.9</v>
@@ -733,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>12</v>
@@ -796,8 +843,8 @@
       <c r="H9" s="9">
         <v>1.3</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>31</v>
+      <c r="I9" s="8">
+        <v>12</v>
       </c>
       <c r="J9" s="8">
         <v>6</v>
@@ -805,7 +852,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>28</v>
@@ -842,6 +889,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -874,14 +922,14 @@
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -889,20 +937,20 @@
         <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="16"/>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="5">
         <v>427.2</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -910,20 +958,20 @@
         <v>19</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5">
         <v>427.2</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -931,7 +979,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="12" t="s">
@@ -988,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>6</v>
@@ -1014,13 +1062,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>6</v>
@@ -1046,13 +1094,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>6</v>
@@ -1115,14 +1163,14 @@
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1130,20 +1178,20 @@
         <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="16"/>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="5">
         <v>360.6</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1151,20 +1199,20 @@
         <v>19</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5">
         <v>344.6</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1172,7 +1220,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="12" t="s">
@@ -1229,7 +1277,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>6</v>
@@ -1255,13 +1303,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>6</v>
@@ -1287,13 +1335,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="C10" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>6</v>

</xml_diff>